<commit_message>
Added v1.1.0 jar file
</commit_message>
<xml_diff>
--- a/resources/api_document/api_doc.xlsx
+++ b/resources/api_document/api_doc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>API_ENDPOINT</t>
   </si>
@@ -126,9 +126,6 @@
 }</t>
   </si>
   <si>
-    <t>http://10.199.240.141:8089/api/questions</t>
-  </si>
-  <si>
     <t>https://int-piapi-internal.stg-openclass.com/tokens</t>
   </si>
   <si>
@@ -138,52 +135,7 @@
 }</t>
   </si>
   <si>
-    <t>Get PI Token</t>
-  </si>
-  <si>
     <t>Get all Questions</t>
-  </si>
-  <si>
-    <t>Create Question</t>
-  </si>
-  <si>
-    <t>{
-  "creatorId": "#creatorId",
-  "creatorPlatform": "#creatorPlatform",
-  "creatoredSource": "#creatoredSource",
-  "creatoredType": "#creatoredType",
-  "deckId": #deckId,
-  "kind": "#kind",
-  "learningObjectives": [
-    "#learningObjectives"
-  ],
-  "question": {
-    "imageUrl": "#imageUrl",
-    "media": "#media",
-    "prompt": "#questionPrompt",
-    "promptType": "#promptType",
-    "timeout": #timeout
-  },
-  "rationale": "#rationale",
-  "stats": {
-    "boxId": #boxId,
-    "correctAttempts": #correctAttempts,
-    "inCorrectAttempts": #inCorrectAttempts,
-    "lastAswered": "#lastAswered",
-    "questionId": #questionId,
-    "skips": #skips,
-    "userId": #userId
-  },
- "correctAnswers": [
-        {
-          "value": "#correctAnswer1",
-          "caseSensitive": #iscorrectAnswer1CaseSensitive
-        }
-  ],
-  "tags": [
-    "#tags"
-  ]
-}</t>
   </si>
   <si>
     <t>Create Expert Deck</t>
@@ -234,6 +186,187 @@
   "title": "#title",
   "updatedAt": "#updatedAt",
   "userId": "#userId"
+}</t>
+  </si>
+  <si>
+    <t>Delete a Question</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>Get a Question</t>
+  </si>
+  <si>
+    <t>Aggregated Text Questions</t>
+  </si>
+  <si>
+    <t>{
+  "deckId": "#deckId", 
+  "question": {
+        "timeout": #timeout,
+        "media": "#media",
+        "imageUrl": "#imageUrl",
+        "promptType": "#promptType"
+    },
+    "stats": {
+        "questionId": #questionId,
+        "userId": #userId,
+        "boxId": #boxId,
+        "skips": #skips,
+        "lastAswered": "#lastAswered",
+        "inCorrectAttempts": #inCorrectAttempts,
+        "correctAttempts": #correctAttempts
+    },
+   "creatorId": "#creatorId",
+    "creatoredType": "#creatoredType",
+    "creatorPlatform": "#creatorPlatform",
+    "creatoredSource": "#creatoredSource",
+"title": "#title", 
+"userId": "#user", 
+"isExpert": #isExpert, 
+"text": "#questionText", 
+"examDate": "#examDate",
+"points":"#points"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tst-piapi-internal.dev-openclass.com/tokens/ </t>
+  </si>
+  <si>
+    <t>Get Staging PI Token</t>
+  </si>
+  <si>
+    <t>Get QA PI Token</t>
+  </si>
+  <si>
+    <t>Image upload through aggregation service</t>
+  </si>
+  <si>
+    <t>Edit Short Answer Type Question</t>
+  </si>
+  <si>
+    <t>Create Short Answer Type Question</t>
+  </si>
+  <si>
+    <t>Create MCQ Type Question</t>
+  </si>
+  <si>
+    <t>{
+  "creatorId": "#creatorId",
+  "creatorPlatform": "#creatorPlatform",
+  "creatoredSource": "#creatoredSource",
+  "creatoredType": "#creatoredType",
+  "deckId": #deckId,
+  "kind": "#kind",
+  "learningObjectives": [
+    "#learningObjectives"
+  ],
+  "question": {
+    "imageUrl": "#imageUrl",
+    "media": "#media",
+    "prompt": "#questionPrompt",
+    "promptType": "#promptType",
+    "timeout": #timeout
+  },
+  "rationale": "#rationale",
+  "stats": {
+    "boxId": #boxId,
+    "correctAttempts": #correctAttempts,
+    "inCorrectAttempts": #inCorrectAttempts,
+    "lastAswered": "#lastAswered",
+    "questionId": #questionId,
+    "skips": #skips,
+    "userId": #userId
+  },
+ "correctAnswers": [
+        #correctAnswerList
+  ],
+  "answers": [
+      {
+        "id": #answer1Id,
+        "value": "#answer1Value",
+        "type": "#answer1Type",
+        "caseSensitive": #answer1CaseSensitive
+      },
+      {
+        "id": #answer2Id,
+        "value": "#answer2Value",
+        "type": "#answer2Type",
+        "caseSensitive": #answer2CaseSensitive
+      },
+      {
+        "id": #answer3Id,
+        "value": "#answer3Value",
+        "type": "#answer3Type",
+        "caseSensitive": #answer3CaseSensitive
+      },
+      {
+        "id": #answer4Id,
+        "value": "#answer4Value",
+        "type": "#answer4Type",
+        "caseSensitive": #answer4CaseSensitive
+      },
+      {
+        "id": #answer5Id,
+        "value": "#answer5Value",
+        "type": "#answer5Type",
+        "caseSensitive": #answer5CaseSensitive
+      }
+    ],
+  "tags": [
+    "#tags"
+  ]
+}</t>
+  </si>
+  <si>
+    <t>http://10.199.253.84:8070/api/questions</t>
+  </si>
+  <si>
+    <t>http://10.199.253.84:8070/api/aggregated_questions/text</t>
+  </si>
+  <si>
+    <t>http://10.199.253.84:8070/api/aggregated_questions/images/upload</t>
+  </si>
+  <si>
+    <t>{
+  "creatorId": "#creatorId",
+  "creatorPlatform": "#creatorPlatform",
+  "creatoredSource": "#creatoredSource",
+  "creatoredType": "#creatoredType",
+  "deckId": #deckId,
+  "kind": "#kind",
+  "learningObjectives": [
+    "#learningObjectives"
+  ],
+  "question": {
+    "imageUrl": "#imageUrl",
+    "media": "#media",
+    "prompt": "#questionPrompt",
+    "promptType": "#promptType",
+    "timeout": #timeout
+  },
+  "rationale": "#rationale",
+  "stats": {
+    "boxId": #boxId,
+    "correctAttempts": #correctAttempts,
+    "inCorrectAttempts": #inCorrectAttempts,
+    "lastAswered": "#lastAswered",
+    "questionId": #questionId,
+    "skips": #skips,
+    "userId": #userId
+  },
+ "answers": [
+        {
+          "id": #correctAnswerId,
+          "value": "#correctAnswerValue",
+          "caseSensitive": #iscorrectAnswerCaseSensitive,
+          "type": "#correctAnswerType"
+        }
+  ],
+  "tags": [
+    "#tags"
+  ]
 }</t>
   </si>
 </sst>
@@ -292,7 +425,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -327,8 +463,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="4"/>
-      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -343,10 +479,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0">
-  <autoFilter ref="A1:D9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D17" totalsRowShown="0">
+  <autoFilter ref="A1:D17"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="API_NAME"/>
+    <tableColumn id="1" name="API_NAME" dataDxfId="3"/>
     <tableColumn id="2" name="API_ENDPOINT" dataDxfId="2"/>
     <tableColumn id="4" name="HTTP_METHOD" dataDxfId="1"/>
     <tableColumn id="3" name="JSON_PAYLOAD_TEMPLATE" dataDxfId="0"/>
@@ -642,23 +778,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D8" sqref="D8"/>
+      <selection pane="topRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
     <col min="4" max="4" width="71.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -672,128 +808,231 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
+      <c r="A2" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
+      <c r="A9" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="D17" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
     <hyperlink ref="B2" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B9" r:id="rId7"/>
+    <hyperlink ref="B13" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B14" r:id="rId10"/>
+    <hyperlink ref="B3" r:id="rId11"/>
+    <hyperlink ref="B15" r:id="rId12"/>
+    <hyperlink ref="B16" r:id="rId13"/>
+    <hyperlink ref="B11" r:id="rId14"/>
+    <hyperlink ref="B12" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>